<commit_message>
Fixed some problems with concentration
</commit_message>
<xml_diff>
--- a/backend/fms_core/tests/valid_templates/Normalization_v3_10_0.xlsx
+++ b/backend/fms_core/tests/valid_templates/Normalization_v3_10_0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sballesteros/Documents/Freezeman/freezeman/backend/fms_core/tests/valid_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84936848-9040-4B45-96CF-1699EEF056B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44FDF9A7-B0A0-E941-84A4-931844B3BF7F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Normalization" sheetId="1" r:id="rId1"/>
     <sheet name="Index" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -2370,7 +2370,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE710"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
@@ -2484,7 +2484,7 @@
         <v>5</v>
       </c>
       <c r="K8" s="19">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="L8" s="19">
         <v>20</v>
@@ -2525,7 +2525,7 @@
         <v>5</v>
       </c>
       <c r="K9" s="25">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="L9" s="25">
         <v>20</v>
@@ -2566,12 +2566,12 @@
         <v>5</v>
       </c>
       <c r="K10" s="25">
-        <v>25</v>
-      </c>
-      <c r="L10" s="25">
-        <v>20</v>
-      </c>
-      <c r="M10" s="25"/>
+        <v>5</v>
+      </c>
+      <c r="L10" s="25"/>
+      <c r="M10" s="25">
+        <v>200</v>
+      </c>
       <c r="N10" s="20" t="s">
         <v>427</v>
       </c>

</xml_diff>

<commit_message>
Added docstring comments and fixed tolerance
</commit_message>
<xml_diff>
--- a/backend/fms_core/tests/valid_templates/Normalization_v3_10_0.xlsx
+++ b/backend/fms_core/tests/valid_templates/Normalization_v3_10_0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sballesteros/Documents/Freezeman/freezeman/backend/fms_core/tests/valid_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC218A7-4BF5-FC4C-907B-CBADCC3DD86F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5758775F-C0F4-F247-ADC0-EC34F20E1AFD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Normalization" sheetId="1" r:id="rId1"/>
     <sheet name="Index" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -2459,7 +2459,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ710"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D1" sqref="A1:D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
@@ -2640,7 +2642,7 @@
         <v>4</v>
       </c>
       <c r="Q8" s="19">
-        <v>12</v>
+        <v>12.5</v>
       </c>
       <c r="R8" s="19"/>
       <c r="S8" s="20" t="s">
@@ -2731,7 +2733,7 @@
       </c>
       <c r="Q10" s="25"/>
       <c r="R10" s="25">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="S10" s="20" t="s">
         <v>426</v>

</xml_diff>